<commit_message>
update wbs and scheduling
Updated versions of WBS and Scheduling due to addition of add and delete user features
A SRS Comments Document
</commit_message>
<xml_diff>
--- a/PM/Schedule/WBS.xlsx
+++ b/PM/Schedule/WBS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\QA\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D049A44F-8275-4EFF-90FB-9E3843F47DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013FE97B-99F4-4151-BA44-D14C83993FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51C8BF43-AD25-4735-ADB6-B04B6DCA29B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Learning hub</t>
   </si>
@@ -143,6 +143,14 @@
   </si>
   <si>
     <t>Logout</t>
+  </si>
+  <si>
+    <t>ADD
+User</t>
+  </si>
+  <si>
+    <t>Delete
+user</t>
   </si>
 </sst>
 </file>
@@ -278,17 +286,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,6 +303,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -317,6 +331,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -326,16 +343,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -939,15 +947,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>587829</xdr:colOff>
+      <xdr:colOff>576943</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>141514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -961,9 +969,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7293429" y="3842657"/>
-          <a:ext cx="32657" cy="10287000"/>
+        <a:xfrm flipH="1">
+          <a:off x="7282543" y="3842657"/>
+          <a:ext cx="10886" cy="12475029"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2431,6 +2439,112 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="1785257" y="12202886"/>
+          <a:ext cx="1284514" cy="10886"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>522514</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>359229</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>587828</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AA06640-3BC3-4A70-BE30-CB0E566C3B1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6008914" y="10755086"/>
+          <a:ext cx="1284514" cy="10885"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABDCE53C-5E42-4863-A1E4-0A94CAB2FA84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6019800" y="11887199"/>
           <a:ext cx="1284514" cy="10886"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2759,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A669D47A-25C9-46DC-BEE1-11EBC62A57ED}">
   <dimension ref="A1:AL72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2798,14 +2912,14 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2825,12 +2939,12 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -2850,12 +2964,12 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2875,12 +2989,12 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2900,12 +3014,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -2994,99 +3108,99 @@
     </row>
     <row r="10" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="9" t="s">
+      <c r="T10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
       <c r="W10" s="1"/>
-      <c r="Z10" s="22" t="s">
+      <c r="Z10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
       <c r="W11" s="1"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
       <c r="W12" s="1"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="22"/>
-      <c r="AB12" s="22"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
@@ -3120,27 +3234,27 @@
     </row>
     <row r="14" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="7"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P14" s="8"/>
+      <c r="P14" s="20"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -3148,41 +3262,41 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="Z14" s="23" t="s">
+      <c r="Z14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AA14" s="22"/>
+      <c r="AA14" s="6"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="14" t="s">
+      <c r="T15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="U15" s="14"/>
+      <c r="U15" s="16"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="Z15" s="22"/>
-      <c r="AA15" s="22"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
     </row>
@@ -3206,8 +3320,8 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="Z16" s="1"/>
@@ -3217,68 +3331,68 @@
     </row>
     <row r="17" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="11"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="18" t="s">
+      <c r="O17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="8"/>
+      <c r="P17" s="20"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="W17" s="1"/>
-      <c r="Z17" s="23" t="s">
+      <c r="Z17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AA17" s="22"/>
+      <c r="AA17" s="6"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
     </row>
     <row r="18" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="U18" s="10"/>
+      <c r="U18" s="9"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
@@ -3302,8 +3416,8 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="Z19" s="1"/>
@@ -3313,27 +3427,27 @@
     </row>
     <row r="20" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="7"/>
+      <c r="J20" s="11"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="19" t="s">
+      <c r="O20" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="P20" s="20"/>
+      <c r="P20" s="23"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -3341,41 +3455,41 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
-      <c r="Z20" s="22" t="s">
+      <c r="Z20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AA20" s="22"/>
+      <c r="AA20" s="6"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
     <row r="21" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="9" t="s">
+      <c r="T21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="U21" s="10"/>
+      <c r="U21" s="9"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
-      <c r="Z21" s="22"/>
-      <c r="AA21" s="22"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
@@ -3399,8 +3513,8 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="Z22" s="1"/>
@@ -3410,19 +3524,19 @@
     </row>
     <row r="23" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="7"/>
+      <c r="J23" s="11"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3443,15 +3557,15 @@
     </row>
     <row r="24" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -3501,19 +3615,19 @@
     </row>
     <row r="26" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="16"/>
+      <c r="J26" s="18"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -3534,15 +3648,15 @@
     </row>
     <row r="27" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -3603,19 +3717,19 @@
     </row>
     <row r="29" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J29" s="7"/>
+      <c r="J29" s="11"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -3647,15 +3761,15 @@
     </row>
     <row r="30" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -3727,19 +3841,19 @@
     </row>
     <row r="32" spans="1:38" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J32" s="7"/>
+      <c r="J32" s="11"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -3771,15 +3885,15 @@
     </row>
     <row r="33" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -3811,8 +3925,8 @@
     </row>
     <row r="34" spans="1:38" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3858,10 +3972,10 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="11" t="s">
+      <c r="I35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="7"/>
+      <c r="J35" s="11"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3900,8 +4014,8 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -3980,10 +4094,10 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="12" t="s">
+      <c r="I38" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J38" s="13"/>
+      <c r="J38" s="15"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -4022,8 +4136,8 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -4102,8 +4216,10 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="I41" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="11"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -4142,8 +4258,8 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -4222,8 +4338,10 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="I44" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J44" s="11"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -4262,8 +4380,8 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -5222,8 +5340,6 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -5262,8 +5378,6 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
@@ -5366,7 +5480,26 @@
       <c r="AL72" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="33">
+    <mergeCell ref="I41:J42"/>
+    <mergeCell ref="I44:J45"/>
+    <mergeCell ref="H2:M6"/>
+    <mergeCell ref="B10:D12"/>
+    <mergeCell ref="I10:K12"/>
+    <mergeCell ref="O10:Q12"/>
+    <mergeCell ref="T10:V12"/>
+    <mergeCell ref="I35:J36"/>
+    <mergeCell ref="I38:J39"/>
+    <mergeCell ref="T15:U16"/>
+    <mergeCell ref="T18:U19"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="I17:J18"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="I23:J24"/>
+    <mergeCell ref="I26:J27"/>
+    <mergeCell ref="O14:P15"/>
+    <mergeCell ref="O17:P18"/>
+    <mergeCell ref="O20:P21"/>
     <mergeCell ref="B32:C34"/>
     <mergeCell ref="Z10:AB12"/>
     <mergeCell ref="Z14:AA15"/>
@@ -5381,23 +5514,6 @@
     <mergeCell ref="B23:C24"/>
     <mergeCell ref="B26:C27"/>
     <mergeCell ref="B29:C30"/>
-    <mergeCell ref="I35:J36"/>
-    <mergeCell ref="I38:J39"/>
-    <mergeCell ref="T15:U16"/>
-    <mergeCell ref="T18:U19"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="I17:J18"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="I23:J24"/>
-    <mergeCell ref="I26:J27"/>
-    <mergeCell ref="O14:P15"/>
-    <mergeCell ref="O17:P18"/>
-    <mergeCell ref="O20:P21"/>
-    <mergeCell ref="H2:M6"/>
-    <mergeCell ref="B10:D12"/>
-    <mergeCell ref="I10:K12"/>
-    <mergeCell ref="O10:Q12"/>
-    <mergeCell ref="T10:V12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>